<commit_message>
update exportação dos resultados  em excel
</commit_message>
<xml_diff>
--- a/teste_Latam.xlsx
+++ b/teste_Latam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dato\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D3051-35B7-41C9-8221-0442BDDEEF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE307D7-22B3-4D58-9533-7B699DF06A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{98DD9042-BC85-4221-A12F-23D7062EFBD5}"/>
   </bookViews>
@@ -54,8 +54,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -83,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF2C7D0-1AC0-4BC7-B0B8-9A6496FDAFBB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,38 +466,8 @@
         <v>12801530</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>570052</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
-      </c>
-      <c r="C3">
-        <v>12801530</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>570052</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
-      </c>
-      <c r="C4">
-        <v>12801530</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>570052</v>
-      </c>
-      <c r="B5">
-        <v>123</v>
-      </c>
-      <c r="C5">
-        <v>12801530</v>
-      </c>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>